<commit_message>
more video parse fixes
</commit_message>
<xml_diff>
--- a/video_parse/louisville_games.xlsx
+++ b/video_parse/louisville_games.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anirudhhaharsha/Desktop/Sports Analytics Projects/Basketball/shot_body_location/data/game_videos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anirudhhaharsha/Desktop/Sports Analytics Projects/Basketball/shot_body_location/new_detector_proj/video_parse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FDDDDB-5C01-DE45-9D44-83FF0036416E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB16162C-DF62-6E44-984C-189A31D61CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9889E7AB-49EA-5841-B4F4-DDC6A300064E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{9889E7AB-49EA-5841-B4F4-DDC6A300064E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,18 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>link</t>
   </si>
   <si>
-    <t>https://youtu.be/3yUZExN61Qw?si=IA6WUrrq3G_LYl7c</t>
-  </si>
-  <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>pitt_louisville_01112025</t>
   </si>
   <si>
     <t>https://youtu.be/jDLvQH0craI?si=CdNatefI7OCcaat9</t>
@@ -482,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1DD2B6A-68C7-8346-ACC5-DAF9EB1B0F19}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,12 +489,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -572,26 +566,18 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>